<commit_message>
FALO PCSS and CLASS plots complete
</commit_message>
<xml_diff>
--- a/data/falo_class.xlsx
+++ b/data/falo_class.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/University of Oregon/BrICC Clinic/BrICC Terms/Spring 2020/pilot_data_2020/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD7C3601-CC3C-FE44-B4BF-DD9199DFB832}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68CEB2EC-CD97-0749-AAFF-0839877AE3DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33940" yWindow="1960" windowWidth="27240" windowHeight="15300" xr2:uid="{0F942E5E-83DD-8A41-8D3E-370346876985}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="22">
   <si>
     <t>Question</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>A lot worse</t>
+  </si>
+  <si>
+    <t>Not worse</t>
   </si>
 </sst>
 </file>
@@ -450,7 +453,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -478,6 +481,9 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
@@ -486,6 +492,9 @@
       <c r="B3" t="s">
         <v>4</v>
       </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
@@ -494,6 +503,9 @@
       <c r="B4" t="s">
         <v>6</v>
       </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
@@ -502,6 +514,9 @@
       <c r="B5" t="s">
         <v>8</v>
       </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
@@ -510,6 +525,9 @@
       <c r="B6" t="s">
         <v>8</v>
       </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
@@ -518,6 +536,9 @@
       <c r="B7" t="s">
         <v>6</v>
       </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
@@ -526,6 +547,9 @@
       <c r="B8" t="s">
         <v>6</v>
       </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
@@ -534,6 +558,9 @@
       <c r="B9" t="s">
         <v>8</v>
       </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
@@ -542,6 +569,9 @@
       <c r="B10" t="s">
         <v>20</v>
       </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
@@ -550,6 +580,9 @@
       <c r="B11" t="s">
         <v>4</v>
       </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
@@ -558,6 +591,9 @@
       <c r="B12" t="s">
         <v>4</v>
       </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
@@ -566,6 +602,9 @@
       <c r="B13" t="s">
         <v>6</v>
       </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
@@ -574,6 +613,9 @@
       <c r="B14" t="s">
         <v>6</v>
       </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
@@ -581,6 +623,9 @@
       </c>
       <c r="B15" t="s">
         <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>